<commit_message>
Etude des livres de Machine Learning - Fichier repère.
</commit_message>
<xml_diff>
--- a/02. Machine learning/Etude des livres.xlsx
+++ b/02. Machine learning/Etude des livres.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Etudié</t>
   </si>
@@ -75,6 +75,18 @@
   </si>
   <si>
     <t>Machine Learning with Python cookbook - Chris Albon</t>
+  </si>
+  <si>
+    <t>Deep Learning Cookbook</t>
+  </si>
+  <si>
+    <t>Hands-On Machine Learning with Scikit-Learn and TensorFlow Concepts</t>
+  </si>
+  <si>
+    <t>Machine Learning for Hackers_ Case Studies and Algorithms to Get You Started [Conway &amp; White 2012-02-25]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Practical Machine Learning and Image Processing For Facial Recognition, Object Detection, and Pattern Recognition Using Python </t>
   </si>
 </sst>
 </file>
@@ -508,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +734,9 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
       <c r="C25" s="1"/>
       <c r="D25" s="7"/>
       <c r="F25" s="10"/>
@@ -805,7 +819,9 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="2"/>
+      <c r="B36" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="C36" s="1"/>
       <c r="D36" s="7"/>
       <c r="F36" s="10"/>
@@ -936,7 +952,9 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
-      <c r="B53" s="2"/>
+      <c r="B53" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="C53" s="1"/>
       <c r="D53" s="7"/>
       <c r="F53" s="10"/>
@@ -1051,7 +1069,9 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
-      <c r="B68" s="2"/>
+      <c r="B68" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="C68" s="1"/>
       <c r="D68" s="7"/>
       <c r="F68" s="10"/>

</xml_diff>